<commit_message>
Change the folding parts in the sheet
</commit_message>
<xml_diff>
--- a/ATDD Scenarios - Extended Text on Assembly Documents.xlsx
+++ b/ATDD Scenarios - Extended Text on Assembly Documents.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/BC TechDays/2025/Session - Testing is Boring^^. Until Now!/AL/AI TT Research 3 lvanvugt - Extended Text on Assembly Documents/Test/atdd.scenarios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/BC TechDays/2025/Session - Testing is Boring^^. Until Now!/BCTD2025_TestingIsBoring_UntilNow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{48DDB92B-08C7-45BE-8218-9E0CCE02F660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B52D00C8-4695-4BE1-9488-97BEEAE0F454}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{48DDB92B-08C7-45BE-8218-9E0CCE02F660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2C3A7D2-AB4F-47D4-865A-329DBD6EC217}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="29" r:id="rId3"/>
+    <pivotCache cacheId="105" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -7233,7 +7233,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{21059AE0-158F-4B62-8618-46A323C28BCD}" name="PivotTable1" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{21059AE0-158F-4B62-8618-46A323C28BCD}" name="PivotTable1" cacheId="105" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showAll="0">
@@ -7622,9 +7622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
   <dimension ref="A1:L411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="8" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E42" sqref="E42"/>
+      <selection pane="topRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7710,7 +7710,7 @@
       </c>
       <c r="L2" s="24"/>
     </row>
-    <row r="3" spans="1:12" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -7840,7 +7840,7 @@
         <v>Then '"Assembly Quote" is not set on Extended Text card page' }</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>Then '"Blanket Assembly Order" is not set on Extended Text card page' }</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>Then '"Assembly Order" is not set on Extended Text card page' }</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>Then '"Assembly Quote" is not set on Extended Text card page' }</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>Then '"Blanket Assembly Order" is not set on Extended Text card page' }</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>Then '"Assembly Order" is not set on Extended Text card page' }</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>20</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>Then '"Assembly Quote" is not set on Extended Text card page' }</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>20</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>Then '"Blanket Assembly Order" is not set on Extended Text card page' }</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="30.75" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>20</v>
       </c>
@@ -8909,7 +8909,7 @@
       </c>
       <c r="L39" s="9"/>
     </row>
-    <row r="40" spans="1:12" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>23</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>Then 'No extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>23</v>
       </c>
@@ -9233,7 +9233,7 @@
         <v>Then 'Extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>23</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>Then 'No extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>23</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>Then 'Extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>23</v>
       </c>
@@ -9699,7 +9699,7 @@
         <v>Then 'No extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>23</v>
       </c>
@@ -9851,7 +9851,7 @@
         <v>Then 'No additional extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>23</v>
       </c>
@@ -10046,7 +10046,7 @@
         <v>Then 'Item is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="31.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>23</v>
       </c>
@@ -10073,7 +10073,7 @@
       </c>
       <c r="L76" s="9"/>
     </row>
-    <row r="77" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>23</v>
       </c>
@@ -10254,7 +10254,7 @@
       </c>
       <c r="L82" s="14"/>
     </row>
-    <row r="83" spans="1:12" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>26</v>
       </c>
@@ -10416,7 +10416,7 @@
         <v>Then 'No extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>26</v>
       </c>
@@ -10578,7 +10578,7 @@
         <v>Then 'Extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>26</v>
       </c>
@@ -10740,7 +10740,7 @@
         <v>Then 'No extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>26</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>Then 'Extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>26</v>
       </c>
@@ -11044,7 +11044,7 @@
         <v>Then 'No extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>26</v>
       </c>
@@ -11196,7 +11196,7 @@
         <v>Then 'No additional extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>26</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>Then 'Item is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="31.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
         <v>26</v>
       </c>
@@ -11418,7 +11418,7 @@
       </c>
       <c r="L119" s="14"/>
     </row>
-    <row r="120" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>26</v>
       </c>
@@ -11599,7 +11599,7 @@
       </c>
       <c r="L125" s="19"/>
     </row>
-    <row r="126" spans="1:12" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>95</v>
       </c>
@@ -11761,7 +11761,7 @@
         <v>Then 'No extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="40.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="40.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>95</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>Then 'Extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>95</v>
       </c>
@@ -12085,7 +12085,7 @@
         <v>Then 'No extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>95</v>
       </c>
@@ -12237,7 +12237,7 @@
         <v>Then 'Extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>95</v>
       </c>
@@ -12389,7 +12389,7 @@
         <v>Then 'No extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>95</v>
       </c>
@@ -12541,7 +12541,7 @@
         <v>Then 'No additional extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>95</v>
       </c>
@@ -12736,7 +12736,7 @@
         <v>Then 'Item is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="31.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A162" s="19" t="s">
         <v>95</v>
       </c>
@@ -12763,7 +12763,7 @@
       </c>
       <c r="L162" s="19"/>
     </row>
-    <row r="163" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
         <v>95</v>
       </c>
@@ -12944,7 +12944,7 @@
       </c>
       <c r="L168" s="29"/>
     </row>
-    <row r="169" spans="1:12" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>23</v>
       </c>
@@ -13106,7 +13106,7 @@
         <v>Then 'No extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>23</v>
       </c>
@@ -13268,7 +13268,7 @@
         <v>Then 'Extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>23</v>
       </c>
@@ -13430,7 +13430,7 @@
         <v>Then 'No extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>23</v>
       </c>
@@ -13582,7 +13582,7 @@
         <v>Then 'Extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>23</v>
       </c>
@@ -13734,7 +13734,7 @@
         <v>Then 'No extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>23</v>
       </c>
@@ -13886,7 +13886,7 @@
         <v>Then 'No additional extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="199" spans="1:12" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" ht="30" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>23</v>
       </c>
@@ -14081,7 +14081,7 @@
         <v>Then 'Resource is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="205" spans="1:12" ht="32.25" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" ht="32.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A205" s="29" t="s">
         <v>23</v>
       </c>
@@ -14108,7 +14108,7 @@
       </c>
       <c r="L205" s="29"/>
     </row>
-    <row r="206" spans="1:12" ht="30.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="3" t="s">
         <v>23</v>
       </c>
@@ -14289,7 +14289,7 @@
       </c>
       <c r="L211" s="32"/>
     </row>
-    <row r="212" spans="1:12" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>26</v>
       </c>
@@ -14451,7 +14451,7 @@
         <v>Then 'No extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="217" spans="1:12" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>26</v>
       </c>
@@ -14613,7 +14613,7 @@
         <v>Then 'Extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="222" spans="1:12" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>26</v>
       </c>
@@ -14775,7 +14775,7 @@
         <v>Then 'No extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>26</v>
       </c>
@@ -14927,7 +14927,7 @@
         <v>Then 'Extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>26</v>
       </c>
@@ -15079,7 +15079,7 @@
         <v>Then 'No extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="237" spans="1:11" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>26</v>
       </c>
@@ -15231,7 +15231,7 @@
         <v>Then 'No additional extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="242" spans="1:12" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" ht="29.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>26</v>
       </c>
@@ -15426,7 +15426,7 @@
         <v>Then 'Resource is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="248" spans="1:12" ht="32.25" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" ht="32.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A248" s="32" t="s">
         <v>26</v>
       </c>
@@ -15453,7 +15453,7 @@
       </c>
       <c r="L248" s="32"/>
     </row>
-    <row r="249" spans="1:12" ht="32.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="3" t="s">
         <v>26</v>
       </c>
@@ -15634,7 +15634,7 @@
       </c>
       <c r="L254" s="35"/>
     </row>
-    <row r="255" spans="1:12" ht="45.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A255" s="3" t="s">
         <v>95</v>
       </c>
@@ -15796,7 +15796,7 @@
         <v>Then 'No extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="260" spans="1:11" ht="27.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" ht="27.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
         <v>95</v>
       </c>
@@ -15958,7 +15958,7 @@
         <v>Then 'Extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="265" spans="1:11" ht="27.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" ht="27.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A265" s="3" t="s">
         <v>95</v>
       </c>
@@ -16120,7 +16120,7 @@
         <v>Then 'No extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="270" spans="1:11" ht="27.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" ht="27.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
         <v>95</v>
       </c>
@@ -16272,7 +16272,7 @@
         <v>Then 'Extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="275" spans="1:11" ht="27.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" ht="27.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A275" s="3" t="s">
         <v>95</v>
       </c>
@@ -16424,7 +16424,7 @@
         <v>Then 'No extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="280" spans="1:11" ht="27.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" ht="27.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A280" s="3" t="s">
         <v>95</v>
       </c>
@@ -16576,7 +16576,7 @@
         <v>Then 'No additional extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="285" spans="1:11" ht="27.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" ht="27.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A285" s="3" t="s">
         <v>95</v>
       </c>
@@ -16771,7 +16771,7 @@
         <v>Then 'Resource is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="291" spans="1:12" ht="31.5" customHeight="1" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" ht="31.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A291" s="35" t="s">
         <v>95</v>
       </c>
@@ -16798,7 +16798,7 @@
       </c>
       <c r="L291" s="35"/>
     </row>
-    <row r="292" spans="1:12" ht="30" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="3" t="s">
         <v>95</v>
       </c>
@@ -16979,7 +16979,7 @@
       </c>
       <c r="L297" s="38"/>
     </row>
-    <row r="298" spans="1:12" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A298" s="3" t="s">
         <v>23</v>
       </c>
@@ -17141,7 +17141,7 @@
         <v>Then 'Extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="303" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
         <v>23</v>
       </c>
@@ -17306,7 +17306,7 @@
         <v>Then 'No extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="308" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A308" s="3" t="s">
         <v>23</v>
       </c>
@@ -17458,7 +17458,7 @@
         <v>Then 'Extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="313" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A313" s="3" t="s">
         <v>23</v>
       </c>
@@ -17610,7 +17610,7 @@
         <v>Then 'No extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="318" spans="1:11" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A318" s="3" t="s">
         <v>23</v>
       </c>
@@ -17762,7 +17762,7 @@
         <v>Then 'No additional extended text lines are added to assembly order' }</v>
       </c>
     </row>
-    <row r="323" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A323" s="3" t="s">
         <v>23</v>
       </c>
@@ -17957,7 +17957,7 @@
         <v>Then 'Text is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="329" spans="1:12" ht="31.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A329" s="38" t="s">
         <v>23</v>
       </c>
@@ -17984,7 +17984,7 @@
       </c>
       <c r="L329" s="38"/>
     </row>
-    <row r="330" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" s="3" t="s">
         <v>23</v>
       </c>
@@ -18165,7 +18165,7 @@
       </c>
       <c r="L335" s="41"/>
     </row>
-    <row r="336" spans="1:12" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A336" s="3" t="s">
         <v>26</v>
       </c>
@@ -18327,7 +18327,7 @@
         <v>Then 'Extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="341" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A341" s="3" t="s">
         <v>26</v>
       </c>
@@ -18492,7 +18492,7 @@
         <v>Then 'No extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="346" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A346" s="3" t="s">
         <v>26</v>
       </c>
@@ -18644,7 +18644,7 @@
         <v>Then 'Extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="351" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
         <v>26</v>
       </c>
@@ -18796,7 +18796,7 @@
         <v>Then 'No extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="356" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A356" s="3" t="s">
         <v>26</v>
       </c>
@@ -18948,7 +18948,7 @@
         <v>Then 'No additional extended text lines are added to assembly quote' }</v>
       </c>
     </row>
-    <row r="361" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A361" s="3" t="s">
         <v>26</v>
       </c>
@@ -19143,7 +19143,7 @@
         <v>Then 'Text is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="367" spans="1:12" ht="31.5" collapsed="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A367" s="41" t="s">
         <v>26</v>
       </c>
@@ -19170,7 +19170,7 @@
       </c>
       <c r="L367" s="41"/>
     </row>
-    <row r="368" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A368" s="3" t="s">
         <v>26</v>
       </c>
@@ -19351,7 +19351,7 @@
       </c>
       <c r="L373" s="57"/>
     </row>
-    <row r="374" spans="1:12" ht="30.75" hidden="1" outlineLevel="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A374" s="3" t="s">
         <v>95</v>
       </c>
@@ -19513,7 +19513,7 @@
         <v>Then 'Extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="379" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A379" s="3" t="s">
         <v>95</v>
       </c>
@@ -19678,7 +19678,7 @@
         <v>Then 'No extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="384" spans="1:12" ht="31.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:12" ht="31.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A384" s="3" t="s">
         <v>95</v>
       </c>
@@ -19830,7 +19830,7 @@
         <v>Then 'Extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="389" spans="1:11" ht="31.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:11" ht="31.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A389" s="3" t="s">
         <v>95</v>
       </c>
@@ -19982,7 +19982,7 @@
         <v>Then 'No extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="394" spans="1:11" ht="31.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:11" ht="31.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A394" s="3" t="s">
         <v>95</v>
       </c>
@@ -20134,7 +20134,7 @@
         <v>Then 'No additional extended text lines are added to blanket assembly order' }</v>
       </c>
     </row>
-    <row r="399" spans="1:11" ht="31.5" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:11" ht="31.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A399" s="3" t="s">
         <v>95</v>
       </c>
@@ -20329,7 +20329,7 @@
         <v>Then 'Text is replaced and extended text lines are removed' } }</v>
       </c>
     </row>
-    <row r="405" spans="1:12" ht="30.75" collapsed="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A405" s="53" t="s">
         <v>95</v>
       </c>
@@ -20356,7 +20356,7 @@
       </c>
       <c r="L405" s="57"/>
     </row>
-    <row r="406" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A406" s="3" t="s">
         <v>95</v>
       </c>

</xml_diff>